<commit_message>
Reading ExcelSheet using loop & 2 Types of Wait
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SITU\OneDrive\Desktop\java_testing\SeleniumBasics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4016CE-786D-4C93-93B0-E711CE71AA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8911710-19EF-47BA-A0A4-C93611A942AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>subrat@gmail.com</t>
+  </si>
+  <si>
+    <t>baivab@gmail.com</t>
+  </si>
+  <si>
+    <t>nayak</t>
+  </si>
+  <si>
+    <t>baivab</t>
   </si>
 </sst>
 </file>
@@ -98,8 +107,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -381,15 +390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -399,7 +408,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -410,7 +419,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -421,16 +430,28 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{23842174-6150-4050-8050-07DD87FD75CE}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{A7444697-6C4E-43DA-9754-CA5012F678ED}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{2B99320A-30BA-4F06-BEEC-F51448D67CA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data Driven Testing FrameWork Course Highlight Added
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SITU\OneDrive\Desktop\java_testing\SeleniumBasics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8911710-19EF-47BA-A0A4-C93611A942AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0345F515-9489-48C6-BB95-D696ED5F2B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Persons" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>firstname</t>
   </si>
@@ -61,6 +62,24 @@
   </si>
   <si>
     <t>baivab</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>mngr5350124</t>
+  </si>
+  <si>
+    <t>qasYnys</t>
+  </si>
+  <si>
+    <t>mngr535012</t>
+  </si>
+  <si>
+    <t>qasYnysp</t>
   </si>
 </sst>
 </file>
@@ -392,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -454,4 +473,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD1025A-62BD-4FF7-A64B-473537A1B08F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>